<commit_message>
push del 17 maggio 22
</commit_message>
<xml_diff>
--- a/heuristic_results.xlsx
+++ b/heuristic_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,26 +589,16 @@
         <v>138.6044</v>
       </c>
       <c r="P2" t="n">
-        <v>138.6044</v>
+        <v>131.3688</v>
       </c>
       <c r="Q2" t="n">
-        <v>138.6044</v>
-      </c>
-      <c r="R2" t="n">
-        <v>138.6044</v>
-      </c>
-      <c r="S2" t="n">
-        <v>138.6044</v>
-      </c>
-      <c r="T2" t="n">
-        <v>138.6044</v>
-      </c>
-      <c r="U2" t="n">
-        <v>138.6044</v>
-      </c>
-      <c r="V2" t="n">
-        <v>138.6044</v>
-      </c>
+        <v>125.6641333333333</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -620,65 +610,51 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>412.5505333333332</v>
+        <v>303.1136</v>
       </c>
       <c r="D3" t="n">
-        <v>398.2831333333334</v>
+        <v>303.1136</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03458339972250634</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K3" t="n">
         <v>25</v>
       </c>
-      <c r="I3" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>8</v>
-      </c>
-      <c r="K3" t="n">
-        <v>60</v>
-      </c>
       <c r="L3" t="n">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="M3" t="n">
-        <v>412.5505333333332</v>
+        <v>303.1136</v>
       </c>
       <c r="N3" t="n">
-        <v>404.3318666666666</v>
+        <v>335.5149333333333</v>
       </c>
       <c r="O3" t="n">
-        <v>414.8926666666665</v>
-      </c>
-      <c r="P3" t="n">
-        <v>398.2831333333334</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>429.7757333333333</v>
-      </c>
-      <c r="R3" t="n">
-        <v>429.7757333333333</v>
-      </c>
-      <c r="S3" t="n">
-        <v>429.7757333333333</v>
-      </c>
-      <c r="T3" t="n">
-        <v>429.7757333333333</v>
-      </c>
-      <c r="U3" t="n">
-        <v>429.7757333333333</v>
-      </c>
-      <c r="V3" t="n">
-        <v>429.7757333333333</v>
-      </c>
+        <v>326.5509333333332</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -690,64 +666,864 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>774.4898666666661</v>
+        <v>249.0065333333333</v>
       </c>
       <c r="D4" t="n">
-        <v>730.4833333333328</v>
+        <v>249.0065333333333</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05682002467344529</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>10</v>
       </c>
       <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
         <v>15</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>25</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" t="n">
+        <v>249.0065333333333</v>
+      </c>
+      <c r="N4" t="n">
+        <v>251.26</v>
+      </c>
+      <c r="O4" t="n">
+        <v>255.0065333333333</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>inst_#4</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>200.1708</v>
+      </c>
+      <c r="D5" t="n">
+        <v>168.6108</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.157665353787865</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>25</v>
+      </c>
+      <c r="L5" t="n">
+        <v>100</v>
+      </c>
+      <c r="M5" t="n">
+        <v>200.1708</v>
+      </c>
+      <c r="N5" t="n">
+        <v>185.836</v>
+      </c>
+      <c r="O5" t="n">
+        <v>168.6108</v>
+      </c>
+      <c r="P5" t="n">
+        <v>174.6108</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>174.6108</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>inst_#5</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>216.0362</v>
+      </c>
+      <c r="D6" t="n">
+        <v>195.8533333333333</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0934235404375133</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>15</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
+        <v>25</v>
+      </c>
+      <c r="L6" t="n">
+        <v>100</v>
+      </c>
+      <c r="M6" t="n">
+        <v>216.0362</v>
+      </c>
+      <c r="N6" t="n">
+        <v>195.8533333333333</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>inst_#6</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>258.0017333333333</v>
+      </c>
+      <c r="D7" t="n">
+        <v>258.0017333333333</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" t="n">
+        <v>25</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" t="n">
+        <v>35</v>
+      </c>
+      <c r="L7" t="n">
+        <v>400</v>
+      </c>
+      <c r="M7" t="n">
+        <v>258.0017333333333</v>
+      </c>
+      <c r="N7" t="n">
+        <v>274.091</v>
+      </c>
+      <c r="O7" t="n">
+        <v>273.6419333333332</v>
+      </c>
+      <c r="P7" t="n">
+        <v>258.7067999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>275.5665999999999</v>
+      </c>
+      <c r="R7" t="n">
+        <v>266.8491999999999</v>
+      </c>
+      <c r="S7" t="n">
+        <v>284.3019999999999</v>
+      </c>
+      <c r="T7" t="n">
+        <v>258.7067999999999</v>
+      </c>
+      <c r="U7" t="n">
+        <v>273.6419333333333</v>
+      </c>
+      <c r="V7" t="n">
+        <v>275.5665999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>inst_#7</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>563.1468</v>
+      </c>
+      <c r="D8" t="n">
+        <v>459.2383999999999</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1845138780864956</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
+      </c>
+      <c r="H8" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>35</v>
+      </c>
+      <c r="L8" t="n">
+        <v>400</v>
+      </c>
+      <c r="M8" t="n">
+        <v>563.1468</v>
+      </c>
+      <c r="N8" t="n">
+        <v>497.0648000000001</v>
+      </c>
+      <c r="O8" t="n">
+        <v>472.7391999999999</v>
+      </c>
+      <c r="P8" t="n">
+        <v>499.4391999999999</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>485.4028</v>
+      </c>
+      <c r="R8" t="n">
+        <v>459.2383999999999</v>
+      </c>
+      <c r="S8" t="n">
+        <v>518.3292</v>
+      </c>
+      <c r="T8" t="n">
+        <v>493.9216</v>
+      </c>
+      <c r="U8" t="n">
+        <v>502.7384000000002</v>
+      </c>
+      <c r="V8" t="n">
+        <v>485.2027999999999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>inst_#8</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>400.6063999999998</v>
+      </c>
+      <c r="D9" t="n">
+        <v>354.4187999999999</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1152942139716189</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>35</v>
+      </c>
+      <c r="L9" t="n">
+        <v>400</v>
+      </c>
+      <c r="M9" t="n">
+        <v>400.6063999999998</v>
+      </c>
+      <c r="N9" t="n">
+        <v>419.8129333333333</v>
+      </c>
+      <c r="O9" t="n">
+        <v>402.5371999999999</v>
+      </c>
+      <c r="P9" t="n">
+        <v>386.7677333333332</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>410.1138666666665</v>
+      </c>
+      <c r="R9" t="n">
+        <v>401.2907999999998</v>
+      </c>
+      <c r="S9" t="n">
+        <v>388.3567999999999</v>
+      </c>
+      <c r="T9" t="n">
+        <v>375.3107999999999</v>
+      </c>
+      <c r="U9" t="n">
+        <v>393.0671999999998</v>
+      </c>
+      <c r="V9" t="n">
+        <v>354.4187999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>inst_#9</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>479.0298666666665</v>
+      </c>
+      <c r="D10" t="n">
+        <v>468.0703999999998</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02287846213625098</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25</v>
+      </c>
+      <c r="I10" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" t="n">
+        <v>35</v>
+      </c>
+      <c r="L10" t="n">
+        <v>400</v>
+      </c>
+      <c r="M10" t="n">
+        <v>479.0298666666665</v>
+      </c>
+      <c r="N10" t="n">
+        <v>478.5618666666666</v>
+      </c>
+      <c r="O10" t="n">
+        <v>489.0329333333332</v>
+      </c>
+      <c r="P10" t="n">
+        <v>468.0703999999998</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>490.0595999999999</v>
+      </c>
+      <c r="R10" t="n">
+        <v>484.1365333333333</v>
+      </c>
+      <c r="S10" t="n">
+        <v>484.1285333333333</v>
+      </c>
+      <c r="T10" t="n">
+        <v>480.4463999999999</v>
+      </c>
+      <c r="U10" t="n">
+        <v>485.7266666666666</v>
+      </c>
+      <c r="V10" t="n">
+        <v>492.3010666666665</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>inst_#10</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>594.2834666666668</v>
+      </c>
+      <c r="D11" t="n">
+        <v>571.3645333333332</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.03856565867781211</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10</v>
+      </c>
+      <c r="H11" t="n">
+        <v>25</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>8</v>
+      </c>
+      <c r="K11" t="n">
+        <v>35</v>
+      </c>
+      <c r="L11" t="n">
+        <v>400</v>
+      </c>
+      <c r="M11" t="n">
+        <v>594.2834666666668</v>
+      </c>
+      <c r="N11" t="n">
+        <v>623.4641333333333</v>
+      </c>
+      <c r="O11" t="n">
+        <v>578.6254666666666</v>
+      </c>
+      <c r="P11" t="n">
+        <v>587.2437333333332</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>582.6306666666665</v>
+      </c>
+      <c r="R11" t="n">
+        <v>577.0391999999999</v>
+      </c>
+      <c r="S11" t="n">
+        <v>587.2437333333332</v>
+      </c>
+      <c r="T11" t="n">
+        <v>578.6254666666666</v>
+      </c>
+      <c r="U11" t="n">
+        <v>582.6306666666665</v>
+      </c>
+      <c r="V11" t="n">
+        <v>571.3645333333332</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>inst_#11</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>617.028933333333</v>
+      </c>
+      <c r="D12" t="n">
+        <v>608.9006666666662</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.01317323423191204</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H12" t="n">
         <v>40</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I12" t="n">
         <v>8</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J12" t="n">
         <v>12</v>
       </c>
-      <c r="K4" t="n">
-        <v>60</v>
-      </c>
-      <c r="L4" t="n">
+      <c r="K12" t="n">
+        <v>50</v>
+      </c>
+      <c r="L12" t="n">
         <v>800</v>
       </c>
-      <c r="M4" t="n">
-        <v>774.4898666666661</v>
-      </c>
-      <c r="N4" t="n">
-        <v>730.4833333333328</v>
-      </c>
-      <c r="O4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="P4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="R4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="S4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="T4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="U4" t="n">
-        <v>742.7650666666663</v>
-      </c>
-      <c r="V4" t="n">
-        <v>742.7650666666663</v>
+      <c r="M12" t="n">
+        <v>617.028933333333</v>
+      </c>
+      <c r="N12" t="n">
+        <v>644.4190666666661</v>
+      </c>
+      <c r="O12" t="n">
+        <v>671.0778666666663</v>
+      </c>
+      <c r="P12" t="n">
+        <v>630.935333333333</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>631.6282666666664</v>
+      </c>
+      <c r="R12" t="n">
+        <v>623.5737333333329</v>
+      </c>
+      <c r="S12" t="n">
+        <v>635.5883999999999</v>
+      </c>
+      <c r="T12" t="n">
+        <v>608.9006666666662</v>
+      </c>
+      <c r="U12" t="n">
+        <v>623.5737333333329</v>
+      </c>
+      <c r="V12" t="n">
+        <v>635.5883999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>inst_#12</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>753.8495999999999</v>
+      </c>
+      <c r="D13" t="n">
+        <v>742.1603999999996</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.01550601074803284</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15</v>
+      </c>
+      <c r="H13" t="n">
+        <v>40</v>
+      </c>
+      <c r="I13" t="n">
+        <v>8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>12</v>
+      </c>
+      <c r="K13" t="n">
+        <v>50</v>
+      </c>
+      <c r="L13" t="n">
+        <v>800</v>
+      </c>
+      <c r="M13" t="n">
+        <v>753.8495999999999</v>
+      </c>
+      <c r="N13" t="n">
+        <v>749.8639999999996</v>
+      </c>
+      <c r="O13" t="n">
+        <v>743.0149333333331</v>
+      </c>
+      <c r="P13" t="n">
+        <v>742.1603999999996</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>757.6237333333329</v>
+      </c>
+      <c r="R13" t="n">
+        <v>754.3286666666663</v>
+      </c>
+      <c r="S13" t="n">
+        <v>755.4022666666663</v>
+      </c>
+      <c r="T13" t="n">
+        <v>744.4525333333329</v>
+      </c>
+      <c r="U13" t="n">
+        <v>770.384933333333</v>
+      </c>
+      <c r="V13" t="n">
+        <v>762.7651999999996</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>inst_#13</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>741.0954666666664</v>
+      </c>
+      <c r="D14" t="n">
+        <v>608.9734666666664</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.1782793255965585</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" t="n">
+        <v>15</v>
+      </c>
+      <c r="H14" t="n">
+        <v>40</v>
+      </c>
+      <c r="I14" t="n">
+        <v>8</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" t="n">
+        <v>50</v>
+      </c>
+      <c r="L14" t="n">
+        <v>800</v>
+      </c>
+      <c r="M14" t="n">
+        <v>741.0954666666664</v>
+      </c>
+      <c r="N14" t="n">
+        <v>660.8802666666663</v>
+      </c>
+      <c r="O14" t="n">
+        <v>624.1794666666664</v>
+      </c>
+      <c r="P14" t="n">
+        <v>666.2049333333329</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>676.9225333333329</v>
+      </c>
+      <c r="R14" t="n">
+        <v>608.9734666666664</v>
+      </c>
+      <c r="S14" t="n">
+        <v>650.7111999999997</v>
+      </c>
+      <c r="T14" t="n">
+        <v>663.0655999999997</v>
+      </c>
+      <c r="U14" t="n">
+        <v>646.308533333333</v>
+      </c>
+      <c r="V14" t="n">
+        <v>643.1962666666664</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>inst_#14</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>724.1653333333329</v>
+      </c>
+      <c r="D15" t="n">
+        <v>698.2141333333329</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.03583601534824458</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" t="n">
+        <v>40</v>
+      </c>
+      <c r="I15" t="n">
+        <v>8</v>
+      </c>
+      <c r="J15" t="n">
+        <v>12</v>
+      </c>
+      <c r="K15" t="n">
+        <v>50</v>
+      </c>
+      <c r="L15" t="n">
+        <v>800</v>
+      </c>
+      <c r="M15" t="n">
+        <v>724.1653333333329</v>
+      </c>
+      <c r="N15" t="n">
+        <v>703.1483999999996</v>
+      </c>
+      <c r="O15" t="n">
+        <v>717.3703999999996</v>
+      </c>
+      <c r="P15" t="n">
+        <v>735.022933333333</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>751.0943999999995</v>
+      </c>
+      <c r="R15" t="n">
+        <v>698.2141333333329</v>
+      </c>
+      <c r="S15" t="n">
+        <v>717.2549333333328</v>
+      </c>
+      <c r="T15" t="n">
+        <v>753.5130666666664</v>
+      </c>
+      <c r="U15" t="n">
+        <v>728.4979999999997</v>
+      </c>
+      <c r="V15" t="n">
+        <v>727.0747999999996</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>inst_#15</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>832.8882666666663</v>
+      </c>
+      <c r="D16" t="n">
+        <v>739.290933333333</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1123768182110702</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="H16" t="n">
+        <v>40</v>
+      </c>
+      <c r="I16" t="n">
+        <v>8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>12</v>
+      </c>
+      <c r="K16" t="n">
+        <v>50</v>
+      </c>
+      <c r="L16" t="n">
+        <v>800</v>
+      </c>
+      <c r="M16" t="n">
+        <v>832.8882666666663</v>
+      </c>
+      <c r="N16" t="n">
+        <v>853.9838666666664</v>
+      </c>
+      <c r="O16" t="n">
+        <v>822.2990666666665</v>
+      </c>
+      <c r="P16" t="n">
+        <v>811.6299999999999</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>876.9778000000001</v>
+      </c>
+      <c r="R16" t="n">
+        <v>806.2107999999997</v>
+      </c>
+      <c r="S16" t="n">
+        <v>739.290933333333</v>
+      </c>
+      <c r="T16" t="n">
+        <v>792.1249333333329</v>
+      </c>
+      <c r="U16" t="n">
+        <v>800.6745333333329</v>
+      </c>
+      <c r="V16" t="n">
+        <v>845.2734666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>